<commit_message>
Pendiente interes laboral y total
</commit_message>
<xml_diff>
--- a/output/Liquidacion_ALARCON_TUCTO_JHOMAYRA.xlsx
+++ b/output/Liquidacion_ALARCON_TUCTO_JHOMAYRA.xlsx
@@ -4646,9 +4646,7 @@
       <c r="AB105" s="159" t="n"/>
       <c r="AC105" s="43" t="n"/>
       <c r="AD105" s="43" t="n"/>
-      <c r="AE105" s="43" t="n">
-        <v>5</v>
-      </c>
+      <c r="AE105" s="43" t="n"/>
       <c r="AF105" s="43" t="n"/>
       <c r="AG105" s="43" t="n"/>
       <c r="AH105" s="43" t="n"/>
@@ -4686,9 +4684,7 @@
       <c r="AB106" s="159" t="n"/>
       <c r="AC106" s="43" t="n"/>
       <c r="AD106" s="43" t="n"/>
-      <c r="AE106" s="43" t="n">
-        <v>15</v>
-      </c>
+      <c r="AE106" s="43" t="n"/>
       <c r="AF106" s="43" t="n"/>
       <c r="AG106" s="43" t="n"/>
       <c r="AH106" s="43" t="n"/>
@@ -4700,7 +4696,11 @@
     </row>
     <row r="107" ht="9.949999999999999" customFormat="1" customHeight="1" s="107">
       <c r="B107" s="43" t="n"/>
-      <c r="D107" s="115" t="n"/>
+      <c r="D107" s="115" t="inlineStr">
+        <is>
+          <t>Por Días</t>
+        </is>
+      </c>
       <c r="F107" s="112" t="n"/>
       <c r="H107" s="129" t="n"/>
       <c r="I107" s="112" t="n"/>
@@ -4727,12 +4727,19 @@
       <c r="B108" s="43" t="n"/>
       <c r="D108" s="115" t="inlineStr">
         <is>
-          <t>Por Meses Completos: 2 mer Tramo</t>
+          <t>49.7 / 30</t>
         </is>
       </c>
       <c r="F108" s="112" t="n"/>
-      <c r="H108" s="129" t="n"/>
+      <c r="H108" s="129" t="n">
+        <v>1.655092592592593</v>
+      </c>
       <c r="I108" s="112" t="n"/>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>15 días</t>
+        </is>
+      </c>
       <c r="K108" s="129" t="n"/>
       <c r="S108" s="110" t="n"/>
       <c r="U108" s="113" t="n"/>
@@ -4742,9 +4749,7 @@
       <c r="AB108" s="159" t="n"/>
       <c r="AC108" s="43" t="n"/>
       <c r="AD108" s="43" t="n"/>
-      <c r="AE108" s="43" t="n">
-        <v>6</v>
-      </c>
+      <c r="AE108" s="43" t="n"/>
       <c r="AF108" s="43" t="n"/>
       <c r="AG108" s="43" t="n"/>
       <c r="AH108" s="43" t="n"/>
@@ -4756,25 +4761,12 @@
     </row>
     <row r="109" ht="9.949999999999999" customFormat="1" customHeight="1" s="107">
       <c r="B109" s="43" t="n"/>
-      <c r="D109" s="115" t="inlineStr">
-        <is>
-          <t>595 / 12</t>
-        </is>
-      </c>
+      <c r="D109" s="115" t="n"/>
       <c r="F109" s="112" t="n"/>
-      <c r="H109" s="129" t="n">
-        <v>49.65277777777778</v>
-      </c>
+      <c r="H109" s="129" t="n"/>
       <c r="I109" s="112" t="n"/>
-      <c r="J109" t="inlineStr">
-        <is>
-          <t>6 meses</t>
-        </is>
-      </c>
       <c r="K109" s="129" t="n"/>
-      <c r="S109" s="110" t="n">
-        <v>297.9166666666667</v>
-      </c>
+      <c r="S109" s="110" t="n"/>
       <c r="U109" s="113" t="n"/>
       <c r="Y109" s="43" t="n"/>
       <c r="Z109" s="43" t="n"/>
@@ -4782,9 +4774,7 @@
       <c r="AB109" s="159" t="n"/>
       <c r="AC109" s="43" t="n"/>
       <c r="AD109" s="43" t="n"/>
-      <c r="AE109" s="43" t="n">
-        <v>0</v>
-      </c>
+      <c r="AE109" s="43" t="n"/>
       <c r="AF109" s="43" t="n"/>
       <c r="AG109" s="43" t="n"/>
       <c r="AH109" s="43" t="n"/>
@@ -4827,7 +4817,11 @@
     </row>
     <row r="111" ht="9.949999999999999" customFormat="1" customHeight="1" s="107">
       <c r="B111" s="43" t="n"/>
-      <c r="D111" s="115" t="n"/>
+      <c r="D111" s="115" t="inlineStr">
+        <is>
+          <t>Por Meses Completos: 2 mer Tramo</t>
+        </is>
+      </c>
       <c r="F111" s="112" t="n"/>
       <c r="H111" s="129" t="n"/>
       <c r="I111" s="112" t="n"/>
@@ -4866,18 +4860,35 @@
     </row>
     <row r="112" ht="9.949999999999999" customFormat="1" customHeight="1" s="107">
       <c r="B112" s="43" t="n"/>
-      <c r="D112" s="115" t="n"/>
+      <c r="D112" s="115" t="inlineStr">
+        <is>
+          <t>595 / 12</t>
+        </is>
+      </c>
       <c r="F112" s="112" t="n"/>
-      <c r="H112" s="129" t="n"/>
+      <c r="H112" s="129" t="n">
+        <v>49.65277777777778</v>
+      </c>
       <c r="I112" s="112" t="n"/>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>6 meses</t>
+        </is>
+      </c>
       <c r="K112" s="129" t="n"/>
-      <c r="S112" s="110" t="n"/>
+      <c r="S112" s="110" t="n">
+        <v>297.9166666666667</v>
+      </c>
       <c r="U112" s="113" t="n"/>
       <c r="Y112" s="43" t="n"/>
     </row>
     <row r="113" ht="9.949999999999999" customFormat="1" customHeight="1" s="107">
       <c r="B113" s="43" t="n"/>
-      <c r="D113" s="115" t="n"/>
+      <c r="D113" s="115" t="inlineStr">
+        <is>
+          <t>Por Días</t>
+        </is>
+      </c>
       <c r="F113" s="112" t="n"/>
       <c r="H113" s="129" t="n"/>
       <c r="I113" s="112" t="n"/>
@@ -4898,10 +4909,21 @@
     </row>
     <row r="114" ht="9.949999999999999" customFormat="1" customHeight="1" s="107">
       <c r="B114" s="43" t="n"/>
-      <c r="D114" s="115" t="n"/>
+      <c r="D114" s="115" t="inlineStr">
+        <is>
+          <t>49.7 / 30</t>
+        </is>
+      </c>
       <c r="F114" s="112" t="n"/>
-      <c r="H114" s="129" t="n"/>
+      <c r="H114" s="129" t="n">
+        <v>1.655092592592593</v>
+      </c>
       <c r="I114" s="112" t="n"/>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>0 días</t>
+        </is>
+      </c>
       <c r="K114" s="129" t="n"/>
       <c r="S114" s="110" t="n"/>
       <c r="U114" s="113" t="n"/>

</xml_diff>